<commit_message>
tbh-report-catalog: add UOMS master data + UOM-based concrete volume + UOM summary analytics
</commit_message>
<xml_diff>
--- a/Projects/tbh-report-catalog/reports/202501 DispatchBilling Verification Pack.xlsx
+++ b/Projects/tbh-report-catalog/reports/202501 DispatchBilling Verification Pack.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="380">
   <si>
     <t>TBH Dispatch / Billing Verification Pack</t>
   </si>
@@ -29,7 +29,7 @@
     <t>Generated</t>
   </si>
   <si>
-    <t>2026-02-17 10:26</t>
+    <t>2026-02-17 10:55</t>
   </si>
   <si>
     <t>Notes</t>
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t>Delivered Qty</t>
+  </si>
+  <si>
+    <t>Concrete Delivered Qty</t>
   </si>
   <si>
     <t>Revenue</t>
@@ -1279,7 +1282,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F53"/>
+  <dimension ref="A1:G53"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1289,8 +1292,9 @@
     <col min="2" max="2" width="9.140625" customWidth="1"/>
     <col min="3" max="3" width="11.93303394317627" customWidth="1"/>
     <col min="4" max="4" width="13.676064491271973" customWidth="1"/>
-    <col min="5" max="5" width="11.700636863708496" customWidth="1"/>
-    <col min="6" max="6" width="11.60714054107666" customWidth="1"/>
+    <col min="5" max="5" width="22.1929874420166" customWidth="1"/>
+    <col min="6" max="6" width="11.700636863708496" customWidth="1"/>
+    <col min="7" max="7" width="11.60714054107666" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1312,24 +1316,30 @@
       <c r="F1" s="3" t="s">
         <v>14</v>
       </c>
+      <c r="G1" s="3" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="4">
         <v>45658</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D2" s="5">
         <v>1.5</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="5">
+        <v>0</v>
+      </c>
+      <c r="F2" s="6">
         <v>99</v>
       </c>
-      <c r="F2" s="0">
+      <c r="G2" s="0">
         <v>1</v>
       </c>
     </row>
@@ -1338,18 +1348,21 @@
         <v>45659</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D3" s="5">
         <v>110.5</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="5">
+        <v>108.5</v>
+      </c>
+      <c r="F3" s="6">
         <v>16701.51</v>
       </c>
-      <c r="F3" s="0">
+      <c r="G3" s="0">
         <v>16</v>
       </c>
     </row>
@@ -1358,18 +1371,21 @@
         <v>45659</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D4" s="5">
         <v>71.5</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="5">
+        <v>71.5</v>
+      </c>
+      <c r="F4" s="6">
         <v>11158.5</v>
       </c>
-      <c r="F4" s="0">
+      <c r="G4" s="0">
         <v>9</v>
       </c>
     </row>
@@ -1378,18 +1394,21 @@
         <v>45659</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D5" s="5">
         <v>216.25</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="5">
+        <v>216.25</v>
+      </c>
+      <c r="F5" s="6">
         <v>33500.51</v>
       </c>
-      <c r="F5" s="0">
+      <c r="G5" s="0">
         <v>31</v>
       </c>
     </row>
@@ -1398,18 +1417,21 @@
         <v>45659</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D6" s="5">
         <v>2.5</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="5">
+        <v>0</v>
+      </c>
+      <c r="F6" s="6">
         <v>100</v>
       </c>
-      <c r="F6" s="0">
+      <c r="G6" s="0">
         <v>2</v>
       </c>
     </row>
@@ -1418,18 +1440,21 @@
         <v>45659</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D7" s="5">
         <v>235</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="5">
+        <v>235</v>
+      </c>
+      <c r="F7" s="6">
         <v>35391.27</v>
       </c>
-      <c r="F7" s="0">
+      <c r="G7" s="0">
         <v>29</v>
       </c>
     </row>
@@ -1438,18 +1463,21 @@
         <v>45660</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D8" s="5">
         <v>124</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="5">
+        <v>124</v>
+      </c>
+      <c r="F8" s="6">
         <v>19397.77</v>
       </c>
-      <c r="F8" s="0">
+      <c r="G8" s="0">
         <v>17</v>
       </c>
     </row>
@@ -1458,18 +1486,21 @@
         <v>45660</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D9" s="5">
         <v>183.25</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="5">
+        <v>183.25</v>
+      </c>
+      <c r="F9" s="6">
         <v>27815.75</v>
       </c>
-      <c r="F9" s="0">
+      <c r="G9" s="0">
         <v>24</v>
       </c>
     </row>
@@ -1478,18 +1509,21 @@
         <v>45660</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D10" s="5">
         <v>436.75</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="5">
+        <v>436.75</v>
+      </c>
+      <c r="F10" s="6">
         <v>67835.69</v>
       </c>
-      <c r="F10" s="0">
+      <c r="G10" s="0">
         <v>56</v>
       </c>
     </row>
@@ -1498,18 +1532,21 @@
         <v>45660</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D11" s="5">
         <v>18</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="5">
+        <v>0</v>
+      </c>
+      <c r="F11" s="6">
         <v>495</v>
       </c>
-      <c r="F11" s="0">
+      <c r="G11" s="0">
         <v>2</v>
       </c>
     </row>
@@ -1518,18 +1555,21 @@
         <v>45660</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D12" s="5">
         <v>19.65</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="5">
+        <v>0</v>
+      </c>
+      <c r="F12" s="6">
         <v>648.45</v>
       </c>
-      <c r="F12" s="0">
+      <c r="G12" s="0">
         <v>1</v>
       </c>
     </row>
@@ -1538,18 +1578,21 @@
         <v>45660</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D13" s="5">
         <v>10</v>
       </c>
-      <c r="E13" s="6">
+      <c r="E13" s="5">
+        <v>0</v>
+      </c>
+      <c r="F13" s="6">
         <v>600</v>
       </c>
-      <c r="F13" s="0">
+      <c r="G13" s="0">
         <v>2</v>
       </c>
     </row>
@@ -1558,18 +1601,21 @@
         <v>45660</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D14" s="5">
         <v>409.25</v>
       </c>
-      <c r="E14" s="6">
+      <c r="E14" s="5">
+        <v>409.25</v>
+      </c>
+      <c r="F14" s="6">
         <v>60660.9</v>
       </c>
-      <c r="F14" s="0">
+      <c r="G14" s="0">
         <v>55</v>
       </c>
     </row>
@@ -1578,18 +1624,21 @@
         <v>45661</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D15" s="5">
         <v>66.5</v>
       </c>
-      <c r="E15" s="6">
+      <c r="E15" s="5">
+        <v>56.5</v>
+      </c>
+      <c r="F15" s="6">
         <v>12335.26</v>
       </c>
-      <c r="F15" s="0">
+      <c r="G15" s="0">
         <v>8</v>
       </c>
     </row>
@@ -1598,18 +1647,21 @@
         <v>45665</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D16" s="5">
         <v>9</v>
       </c>
-      <c r="E16" s="6">
+      <c r="E16" s="5">
+        <v>9</v>
+      </c>
+      <c r="F16" s="6">
         <v>1647</v>
       </c>
-      <c r="F16" s="0">
+      <c r="G16" s="0">
         <v>1</v>
       </c>
     </row>
@@ -1618,18 +1670,21 @@
         <v>45665</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D17" s="5">
         <v>44</v>
       </c>
-      <c r="E17" s="6">
+      <c r="E17" s="5">
+        <v>44</v>
+      </c>
+      <c r="F17" s="6">
         <v>7264</v>
       </c>
-      <c r="F17" s="0">
+      <c r="G17" s="0">
         <v>5</v>
       </c>
     </row>
@@ -1638,18 +1693,21 @@
         <v>45665</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D18" s="5">
         <v>39</v>
       </c>
-      <c r="E18" s="6">
+      <c r="E18" s="5">
+        <v>39</v>
+      </c>
+      <c r="F18" s="6">
         <v>6957.5</v>
       </c>
-      <c r="F18" s="0">
+      <c r="G18" s="0">
         <v>7</v>
       </c>
     </row>
@@ -1658,18 +1716,21 @@
         <v>45666</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D19" s="5">
         <v>45.5</v>
       </c>
-      <c r="E19" s="6">
+      <c r="E19" s="5">
+        <v>45.5</v>
+      </c>
+      <c r="F19" s="6">
         <v>7837</v>
       </c>
-      <c r="F19" s="0">
+      <c r="G19" s="0">
         <v>7</v>
       </c>
     </row>
@@ -1678,18 +1739,21 @@
         <v>45666</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D20" s="5">
         <v>102</v>
       </c>
-      <c r="E20" s="6">
+      <c r="E20" s="5">
+        <v>102</v>
+      </c>
+      <c r="F20" s="6">
         <v>15643</v>
       </c>
-      <c r="F20" s="0">
+      <c r="G20" s="0">
         <v>12</v>
       </c>
     </row>
@@ -1698,18 +1762,21 @@
         <v>45666</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D21" s="5">
         <v>128</v>
       </c>
-      <c r="E21" s="6">
+      <c r="E21" s="5">
+        <v>128</v>
+      </c>
+      <c r="F21" s="6">
         <v>18905.5</v>
       </c>
-      <c r="F21" s="0">
+      <c r="G21" s="0">
         <v>15</v>
       </c>
     </row>
@@ -1718,18 +1785,21 @@
         <v>45666</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D22" s="5">
         <v>10</v>
       </c>
-      <c r="E22" s="6">
+      <c r="E22" s="5">
+        <v>0</v>
+      </c>
+      <c r="F22" s="6">
         <v>600</v>
       </c>
-      <c r="F22" s="0">
+      <c r="G22" s="0">
         <v>1</v>
       </c>
     </row>
@@ -1738,18 +1808,21 @@
         <v>45666</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D23" s="5">
         <v>75</v>
       </c>
-      <c r="E23" s="6">
+      <c r="E23" s="5">
+        <v>75</v>
+      </c>
+      <c r="F23" s="6">
         <v>12519</v>
       </c>
-      <c r="F23" s="0">
+      <c r="G23" s="0">
         <v>11</v>
       </c>
     </row>
@@ -1758,18 +1831,21 @@
         <v>45667</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D24" s="5">
         <v>105</v>
       </c>
-      <c r="E24" s="6">
+      <c r="E24" s="5">
+        <v>105</v>
+      </c>
+      <c r="F24" s="6">
         <v>16723.27</v>
       </c>
-      <c r="F24" s="0">
+      <c r="G24" s="0">
         <v>13</v>
       </c>
     </row>
@@ -1778,18 +1854,21 @@
         <v>45667</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D25" s="5">
         <v>226</v>
       </c>
-      <c r="E25" s="6">
+      <c r="E25" s="5">
+        <v>226</v>
+      </c>
+      <c r="F25" s="6">
         <v>32755.52</v>
       </c>
-      <c r="F25" s="0">
+      <c r="G25" s="0">
         <v>28</v>
       </c>
     </row>
@@ -1798,18 +1877,21 @@
         <v>45667</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D26" s="5">
         <v>362</v>
       </c>
-      <c r="E26" s="6">
+      <c r="E26" s="5">
+        <v>362</v>
+      </c>
+      <c r="F26" s="6">
         <v>54744.91</v>
       </c>
-      <c r="F26" s="0">
+      <c r="G26" s="0">
         <v>41</v>
       </c>
     </row>
@@ -1818,18 +1900,21 @@
         <v>45667</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D27" s="5">
         <v>2</v>
       </c>
-      <c r="E27" s="6">
+      <c r="E27" s="5">
+        <v>0</v>
+      </c>
+      <c r="F27" s="6">
         <v>61</v>
       </c>
-      <c r="F27" s="0">
+      <c r="G27" s="0">
         <v>1</v>
       </c>
     </row>
@@ -1838,18 +1923,21 @@
         <v>45667</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D28" s="5">
         <v>344.75</v>
       </c>
-      <c r="E28" s="6">
+      <c r="E28" s="5">
+        <v>344.75</v>
+      </c>
+      <c r="F28" s="6">
         <v>53881.41</v>
       </c>
-      <c r="F28" s="0">
+      <c r="G28" s="0">
         <v>41</v>
       </c>
     </row>
@@ -1858,18 +1946,21 @@
         <v>45670</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D29" s="5">
         <v>113.5</v>
       </c>
-      <c r="E29" s="6">
+      <c r="E29" s="5">
+        <v>112.5</v>
+      </c>
+      <c r="F29" s="6">
         <v>18138.25</v>
       </c>
-      <c r="F29" s="0">
+      <c r="G29" s="0">
         <v>16</v>
       </c>
     </row>
@@ -1878,18 +1969,21 @@
         <v>45670</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D30" s="5">
         <v>433.25</v>
       </c>
-      <c r="E30" s="6">
+      <c r="E30" s="5">
+        <v>433.25</v>
+      </c>
+      <c r="F30" s="6">
         <v>62617.88</v>
       </c>
-      <c r="F30" s="0">
+      <c r="G30" s="0">
         <v>50</v>
       </c>
     </row>
@@ -1898,18 +1992,21 @@
         <v>45670</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D31" s="5">
         <v>657.25</v>
       </c>
-      <c r="E31" s="6">
+      <c r="E31" s="5">
+        <v>657.25</v>
+      </c>
+      <c r="F31" s="6">
         <v>98735.64</v>
       </c>
-      <c r="F31" s="0">
+      <c r="G31" s="0">
         <v>77</v>
       </c>
     </row>
@@ -1918,18 +2015,21 @@
         <v>45670</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D32" s="5">
         <v>9</v>
       </c>
-      <c r="E32" s="6">
+      <c r="E32" s="5">
+        <v>0</v>
+      </c>
+      <c r="F32" s="6">
         <v>321</v>
       </c>
-      <c r="F32" s="0">
+      <c r="G32" s="0">
         <v>2</v>
       </c>
     </row>
@@ -1938,18 +2038,21 @@
         <v>45670</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D33" s="5">
         <v>282</v>
       </c>
-      <c r="E33" s="6">
+      <c r="E33" s="5">
+        <v>282</v>
+      </c>
+      <c r="F33" s="6">
         <v>42290.75</v>
       </c>
-      <c r="F33" s="0">
+      <c r="G33" s="0">
         <v>35</v>
       </c>
     </row>
@@ -1958,18 +2061,21 @@
         <v>45671</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D34" s="5">
         <v>54.5</v>
       </c>
-      <c r="E34" s="6">
+      <c r="E34" s="5">
+        <v>54.5</v>
+      </c>
+      <c r="F34" s="6">
         <v>8279.75</v>
       </c>
-      <c r="F34" s="0">
+      <c r="G34" s="0">
         <v>7</v>
       </c>
     </row>
@@ -1978,18 +2084,21 @@
         <v>45671</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D35" s="5">
         <v>110.5</v>
       </c>
-      <c r="E35" s="6">
+      <c r="E35" s="5">
+        <v>110.5</v>
+      </c>
+      <c r="F35" s="6">
         <v>15859</v>
       </c>
-      <c r="F35" s="0">
+      <c r="G35" s="0">
         <v>13</v>
       </c>
     </row>
@@ -1998,18 +2107,21 @@
         <v>45671</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D36" s="5">
         <v>126.5</v>
       </c>
-      <c r="E36" s="6">
+      <c r="E36" s="5">
+        <v>126.5</v>
+      </c>
+      <c r="F36" s="6">
         <v>19296.76</v>
       </c>
-      <c r="F36" s="0">
+      <c r="G36" s="0">
         <v>17</v>
       </c>
     </row>
@@ -2018,18 +2130,21 @@
         <v>45671</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D37" s="5">
         <v>18</v>
       </c>
-      <c r="E37" s="6">
+      <c r="E37" s="5">
+        <v>0</v>
+      </c>
+      <c r="F37" s="6">
         <v>600</v>
       </c>
-      <c r="F37" s="0">
+      <c r="G37" s="0">
         <v>2</v>
       </c>
     </row>
@@ -2038,18 +2153,21 @@
         <v>45671</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D38" s="5">
         <v>159</v>
       </c>
-      <c r="E38" s="6">
+      <c r="E38" s="5">
+        <v>159</v>
+      </c>
+      <c r="F38" s="6">
         <v>25177.51</v>
       </c>
-      <c r="F38" s="0">
+      <c r="G38" s="0">
         <v>23</v>
       </c>
     </row>
@@ -2058,18 +2176,21 @@
         <v>45672</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D39" s="5">
         <v>112.25</v>
       </c>
-      <c r="E39" s="6">
+      <c r="E39" s="5">
+        <v>111.25</v>
+      </c>
+      <c r="F39" s="6">
         <v>18174.26</v>
       </c>
-      <c r="F39" s="0">
+      <c r="G39" s="0">
         <v>16</v>
       </c>
     </row>
@@ -2078,18 +2199,21 @@
         <v>45672</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D40" s="5">
         <v>51.5</v>
       </c>
-      <c r="E40" s="6">
+      <c r="E40" s="5">
+        <v>51.5</v>
+      </c>
+      <c r="F40" s="6">
         <v>7016</v>
       </c>
-      <c r="F40" s="0">
+      <c r="G40" s="0">
         <v>6</v>
       </c>
     </row>
@@ -2098,18 +2222,21 @@
         <v>45672</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D41" s="5">
         <v>280.75</v>
       </c>
-      <c r="E41" s="6">
+      <c r="E41" s="5">
+        <v>280.75</v>
+      </c>
+      <c r="F41" s="6">
         <v>43232</v>
       </c>
-      <c r="F41" s="0">
+      <c r="G41" s="0">
         <v>35</v>
       </c>
     </row>
@@ -2118,18 +2245,21 @@
         <v>45672</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D42" s="5">
         <v>5</v>
       </c>
-      <c r="E42" s="6">
+      <c r="E42" s="5">
+        <v>0</v>
+      </c>
+      <c r="F42" s="6">
         <v>316.5</v>
       </c>
-      <c r="F42" s="0">
+      <c r="G42" s="0">
         <v>2</v>
       </c>
     </row>
@@ -2138,18 +2268,21 @@
         <v>45672</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D43" s="5">
         <v>22</v>
       </c>
-      <c r="E43" s="6">
+      <c r="E43" s="5">
+        <v>0</v>
+      </c>
+      <c r="F43" s="6">
         <v>806</v>
       </c>
-      <c r="F43" s="0">
+      <c r="G43" s="0">
         <v>2</v>
       </c>
     </row>
@@ -2158,18 +2291,21 @@
         <v>45672</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D44" s="5">
         <v>191.5</v>
       </c>
-      <c r="E44" s="6">
+      <c r="E44" s="5">
+        <v>155.5</v>
+      </c>
+      <c r="F44" s="6">
         <v>25606.75</v>
       </c>
-      <c r="F44" s="0">
+      <c r="G44" s="0">
         <v>23</v>
       </c>
     </row>
@@ -2178,18 +2314,21 @@
         <v>45673</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D45" s="5">
         <v>23</v>
       </c>
-      <c r="E45" s="6">
+      <c r="E45" s="5">
+        <v>23</v>
+      </c>
+      <c r="F45" s="6">
         <v>3952.5</v>
       </c>
-      <c r="F45" s="0">
+      <c r="G45" s="0">
         <v>5</v>
       </c>
     </row>
@@ -2198,18 +2337,21 @@
         <v>45673</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D46" s="5">
         <v>46.5</v>
       </c>
-      <c r="E46" s="6">
+      <c r="E46" s="5">
+        <v>46.5</v>
+      </c>
+      <c r="F46" s="6">
         <v>7880</v>
       </c>
-      <c r="F46" s="0">
+      <c r="G46" s="0">
         <v>7</v>
       </c>
     </row>
@@ -2218,18 +2360,21 @@
         <v>45673</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D47" s="5">
         <v>323.5</v>
       </c>
-      <c r="E47" s="6">
+      <c r="E47" s="5">
+        <v>323.5</v>
+      </c>
+      <c r="F47" s="6">
         <v>49572.26</v>
       </c>
-      <c r="F47" s="0">
+      <c r="G47" s="0">
         <v>41</v>
       </c>
     </row>
@@ -2238,18 +2383,21 @@
         <v>45673</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D48" s="5">
         <v>48.81</v>
       </c>
-      <c r="E48" s="6">
+      <c r="E48" s="5">
+        <v>0</v>
+      </c>
+      <c r="F48" s="6">
         <v>1989.66</v>
       </c>
-      <c r="F48" s="0">
+      <c r="G48" s="0">
         <v>4</v>
       </c>
     </row>
@@ -2258,18 +2406,21 @@
         <v>45673</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D49" s="5">
         <v>343</v>
       </c>
-      <c r="E49" s="6">
+      <c r="E49" s="5">
+        <v>343</v>
+      </c>
+      <c r="F49" s="6">
         <v>53579.01</v>
       </c>
-      <c r="F49" s="0">
+      <c r="G49" s="0">
         <v>41</v>
       </c>
     </row>
@@ -2278,18 +2429,21 @@
         <v>45674</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D50" s="5">
         <v>110.5</v>
       </c>
-      <c r="E50" s="6">
+      <c r="E50" s="5">
+        <v>109.5</v>
+      </c>
+      <c r="F50" s="6">
         <v>18287.5</v>
       </c>
-      <c r="F50" s="0">
+      <c r="G50" s="0">
         <v>14</v>
       </c>
     </row>
@@ -2298,18 +2452,21 @@
         <v>45674</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D51" s="5">
         <v>31.5</v>
       </c>
-      <c r="E51" s="6">
+      <c r="E51" s="5">
+        <v>31.5</v>
+      </c>
+      <c r="F51" s="6">
         <v>5682</v>
       </c>
-      <c r="F51" s="0">
+      <c r="G51" s="0">
         <v>4</v>
       </c>
     </row>
@@ -2318,18 +2475,21 @@
         <v>45674</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D52" s="5">
         <v>496.25</v>
       </c>
-      <c r="E52" s="6">
+      <c r="E52" s="5">
+        <v>496.25</v>
+      </c>
+      <c r="F52" s="6">
         <v>71187.38</v>
       </c>
-      <c r="F52" s="0">
+      <c r="G52" s="0">
         <v>55</v>
       </c>
     </row>
@@ -2338,18 +2498,21 @@
         <v>45674</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D53" s="5">
         <v>535.25</v>
       </c>
-      <c r="E53" s="6">
+      <c r="E53" s="5">
+        <v>535.25</v>
+      </c>
+      <c r="F53" s="6">
         <v>87467.26</v>
       </c>
-      <c r="F53" s="0">
+      <c r="G53" s="0">
         <v>67</v>
       </c>
     </row>
@@ -2360,7 +2523,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2371,13 +2534,14 @@
     <col min="3" max="3" width="9.140625" customWidth="1"/>
     <col min="4" max="4" width="11.93303394317627" customWidth="1"/>
     <col min="5" max="5" width="13.676064491271973" customWidth="1"/>
-    <col min="6" max="6" width="12.677665710449219" customWidth="1"/>
-    <col min="7" max="7" width="11.60714054107666" customWidth="1"/>
+    <col min="6" max="6" width="22.1929874420166" customWidth="1"/>
+    <col min="7" max="7" width="12.677665710449219" customWidth="1"/>
+    <col min="8" max="8" width="11.60714054107666" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -2396,6 +2560,9 @@
       </c>
       <c r="G1" s="3" t="s">
         <v>14</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="2">
@@ -2406,18 +2573,21 @@
         <v>1</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E2" s="5">
         <v>807.75</v>
       </c>
-      <c r="F2" s="6">
+      <c r="F2" s="5">
+        <v>802.75</v>
+      </c>
+      <c r="G2" s="6">
         <v>129138.81</v>
       </c>
-      <c r="G2" s="0">
+      <c r="H2" s="0">
         <v>112</v>
       </c>
     </row>
@@ -2429,18 +2599,21 @@
         <v>1</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E3" s="5">
         <v>1300</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="5">
+        <v>1300</v>
+      </c>
+      <c r="G3" s="6">
         <v>193691.65</v>
       </c>
-      <c r="G3" s="0">
+      <c r="H3" s="0">
         <v>158</v>
       </c>
     </row>
@@ -2452,18 +2625,21 @@
         <v>1</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E4" s="5">
         <v>3093.75</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="5">
+        <v>3083.75</v>
+      </c>
+      <c r="G4" s="6">
         <v>469345.91</v>
       </c>
-      <c r="G4" s="0">
+      <c r="H4" s="0">
         <v>376</v>
       </c>
     </row>
@@ -2475,18 +2651,21 @@
         <v>1</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E5" s="5">
         <v>54</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="5">
+        <v>0</v>
+      </c>
+      <c r="G5" s="6">
         <v>1931.5</v>
       </c>
-      <c r="G5" s="0">
+      <c r="H5" s="0">
         <v>11</v>
       </c>
     </row>
@@ -2498,18 +2677,21 @@
         <v>1</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E6" s="5">
         <v>19.65</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="5">
+        <v>0</v>
+      </c>
+      <c r="G6" s="6">
         <v>648.45</v>
       </c>
-      <c r="G6" s="0">
+      <c r="H6" s="0">
         <v>1</v>
       </c>
     </row>
@@ -2521,18 +2703,21 @@
         <v>1</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E7" s="5">
         <v>20</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="5">
+        <v>0</v>
+      </c>
+      <c r="G7" s="6">
         <v>1200</v>
       </c>
-      <c r="G7" s="0">
+      <c r="H7" s="0">
         <v>3</v>
       </c>
     </row>
@@ -2544,18 +2729,21 @@
         <v>1</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E8" s="5">
         <v>72.81</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="5">
+        <v>0</v>
+      </c>
+      <c r="G8" s="6">
         <v>2856.66</v>
       </c>
-      <c r="G8" s="0">
+      <c r="H8" s="0">
         <v>7</v>
       </c>
     </row>
@@ -2567,18 +2755,21 @@
         <v>1</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E9" s="5">
         <v>2613.75</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F9" s="5">
+        <v>2577.75</v>
+      </c>
+      <c r="G9" s="6">
         <v>403531.36</v>
       </c>
-      <c r="G9" s="0">
+      <c r="H9" s="0">
         <v>332</v>
       </c>
     </row>
@@ -2603,21 +2794,21 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B2" s="6">
         <v>1647</v>
@@ -2631,7 +2822,7 @@
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B3" s="6">
         <v>3825</v>
@@ -2645,7 +2836,7 @@
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B4" s="6">
         <v>286</v>
@@ -2659,7 +2850,7 @@
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B5" s="6">
         <v>3439</v>
@@ -2673,7 +2864,7 @@
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B6" s="6">
         <v>2520</v>
@@ -2687,7 +2878,7 @@
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B7" s="6">
         <v>3971</v>
@@ -2701,7 +2892,7 @@
     </row>
     <row r="8">
       <c r="A8" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B8" s="6">
         <v>180.5</v>
@@ -2715,7 +2906,7 @@
     </row>
     <row r="9">
       <c r="A9" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B9" s="6">
         <v>4713</v>
@@ -2729,7 +2920,7 @@
     </row>
     <row r="10">
       <c r="A10" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B10" s="6">
         <v>562.5</v>
@@ -2743,7 +2934,7 @@
     </row>
     <row r="11">
       <c r="A11" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B11" s="6">
         <v>1738.5</v>
@@ -2757,7 +2948,7 @@
     </row>
     <row r="12">
       <c r="A12" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B12" s="6">
         <v>425</v>
@@ -2771,7 +2962,7 @@
     </row>
     <row r="13">
       <c r="A13" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B13" s="6">
         <v>600</v>
@@ -2785,7 +2976,7 @@
     </row>
     <row r="14">
       <c r="A14" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B14" s="6">
         <v>6006</v>
@@ -2799,7 +2990,7 @@
     </row>
     <row r="15">
       <c r="A15" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B15" s="6">
         <v>4332</v>
@@ -2813,7 +3004,7 @@
     </row>
     <row r="16">
       <c r="A16" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B16" s="6">
         <v>11311</v>
@@ -2827,7 +3018,7 @@
     </row>
     <row r="17">
       <c r="A17" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B17" s="6">
         <v>2483</v>
@@ -2841,7 +3032,7 @@
     </row>
     <row r="18">
       <c r="A18" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B18" s="6">
         <v>255</v>
@@ -2855,7 +3046,7 @@
     </row>
     <row r="19">
       <c r="A19" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B19" s="6">
         <v>1800</v>
@@ -2869,7 +3060,7 @@
     </row>
     <row r="20">
       <c r="A20" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B20" s="6">
         <v>2935.5</v>
@@ -2883,7 +3074,7 @@
     </row>
     <row r="21">
       <c r="A21" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B21" s="6">
         <v>8791</v>
@@ -2897,7 +3088,7 @@
     </row>
     <row r="22">
       <c r="A22" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B22" s="6">
         <v>6721</v>
@@ -2911,7 +3102,7 @@
     </row>
     <row r="23">
       <c r="A23" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B23" s="6">
         <v>8078.5</v>
@@ -2925,7 +3116,7 @@
     </row>
     <row r="24">
       <c r="A24" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B24" s="6">
         <v>382</v>
@@ -2939,7 +3130,7 @@
     </row>
     <row r="25">
       <c r="A25" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B25" s="6">
         <v>803.25</v>
@@ -2953,7 +3144,7 @@
     </row>
     <row r="26">
       <c r="A26" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B26" s="6">
         <v>1715</v>
@@ -2967,7 +3158,7 @@
     </row>
     <row r="27">
       <c r="A27" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B27" s="6">
         <v>499.5</v>
@@ -2981,7 +3172,7 @@
     </row>
     <row r="28">
       <c r="A28" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B28" s="6">
         <v>4162.5</v>
@@ -2995,7 +3186,7 @@
     </row>
     <row r="29">
       <c r="A29" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B29" s="6">
         <v>3496.5</v>
@@ -3009,7 +3200,7 @@
     </row>
     <row r="30">
       <c r="A30" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B30" s="6">
         <v>810</v>
@@ -3023,7 +3214,7 @@
     </row>
     <row r="31">
       <c r="A31" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B31" s="6">
         <v>635.25</v>
@@ -3037,7 +3228,7 @@
     </row>
     <row r="32">
       <c r="A32" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B32" s="6">
         <v>1349</v>
@@ -3051,7 +3242,7 @@
     </row>
     <row r="33">
       <c r="A33" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B33" s="6">
         <v>145</v>
@@ -3065,7 +3256,7 @@
     </row>
     <row r="34">
       <c r="A34" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B34" s="6">
         <v>1184</v>
@@ -3079,7 +3270,7 @@
     </row>
     <row r="35">
       <c r="A35" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B35" s="6">
         <v>1396.5</v>
@@ -3093,7 +3284,7 @@
     </row>
     <row r="36">
       <c r="A36" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B36" s="6">
         <v>2888</v>
@@ -3107,7 +3298,7 @@
     </row>
     <row r="37">
       <c r="A37" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B37" s="6">
         <v>2743.5</v>
@@ -3121,7 +3312,7 @@
     </row>
     <row r="38">
       <c r="A38" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B38" s="6">
         <v>2839</v>
@@ -3135,7 +3326,7 @@
     </row>
     <row r="39">
       <c r="A39" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B39" s="6">
         <v>41782.63</v>
@@ -3149,7 +3340,7 @@
     </row>
     <row r="40">
       <c r="A40" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B40" s="6">
         <v>3302.25</v>
@@ -3163,7 +3354,7 @@
     </row>
     <row r="41">
       <c r="A41" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B41" s="6">
         <v>5130</v>
@@ -3177,7 +3368,7 @@
     </row>
     <row r="42">
       <c r="A42" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B42" s="6">
         <v>292</v>
@@ -3191,7 +3382,7 @@
     </row>
     <row r="43">
       <c r="A43" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B43" s="6">
         <v>5534.25</v>
@@ -3205,7 +3396,7 @@
     </row>
     <row r="44">
       <c r="A44" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B44" s="6">
         <v>357</v>
@@ -3219,7 +3410,7 @@
     </row>
     <row r="45">
       <c r="A45" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B45" s="6">
         <v>12249</v>
@@ -3233,7 +3424,7 @@
     </row>
     <row r="46">
       <c r="A46" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B46" s="6">
         <v>2227.5</v>
@@ -3247,7 +3438,7 @@
     </row>
     <row r="47">
       <c r="A47" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B47" s="6">
         <v>4185.5</v>
@@ -3261,7 +3452,7 @@
     </row>
     <row r="48">
       <c r="A48" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B48" s="6">
         <v>11924</v>
@@ -3275,7 +3466,7 @@
     </row>
     <row r="49">
       <c r="A49" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B49" s="6">
         <v>1530</v>
@@ -3289,7 +3480,7 @@
     </row>
     <row r="50">
       <c r="A50" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B50" s="6">
         <v>1300.5</v>
@@ -3303,7 +3494,7 @@
     </row>
     <row r="51">
       <c r="A51" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B51" s="6">
         <v>55</v>
@@ -3317,7 +3508,7 @@
     </row>
     <row r="52">
       <c r="A52" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B52" s="6">
         <v>266</v>
@@ -3331,7 +3522,7 @@
     </row>
     <row r="53">
       <c r="A53" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B53" s="6">
         <v>5043.5</v>
@@ -3345,7 +3536,7 @@
     </row>
     <row r="54">
       <c r="A54" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B54" s="6">
         <v>1211</v>
@@ -3359,7 +3550,7 @@
     </row>
     <row r="55">
       <c r="A55" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B55" s="6">
         <v>3193.5</v>
@@ -3373,7 +3564,7 @@
     </row>
     <row r="56">
       <c r="A56" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B56" s="6">
         <v>900</v>
@@ -3387,7 +3578,7 @@
     </row>
     <row r="57">
       <c r="A57" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B57" s="6">
         <v>2270.75</v>
@@ -3401,7 +3592,7 @@
     </row>
     <row r="58">
       <c r="A58" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B58" s="6">
         <v>277.5</v>
@@ -3415,7 +3606,7 @@
     </row>
     <row r="59">
       <c r="A59" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B59" s="6">
         <v>3312</v>
@@ -3429,7 +3620,7 @@
     </row>
     <row r="60">
       <c r="A60" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B60" s="6">
         <v>450</v>
@@ -3443,7 +3634,7 @@
     </row>
     <row r="61">
       <c r="A61" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B61" s="6">
         <v>4094</v>
@@ -3457,7 +3648,7 @@
     </row>
     <row r="62">
       <c r="A62" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B62" s="6">
         <v>2118</v>
@@ -3471,7 +3662,7 @@
     </row>
     <row r="63">
       <c r="A63" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B63" s="6">
         <v>80</v>
@@ -3485,7 +3676,7 @@
     </row>
     <row r="64">
       <c r="A64" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B64" s="6">
         <v>4246.5</v>
@@ -3499,7 +3690,7 @@
     </row>
     <row r="65">
       <c r="A65" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B65" s="6">
         <v>2755</v>
@@ -3513,7 +3704,7 @@
     </row>
     <row r="66">
       <c r="A66" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B66" s="6">
         <v>4531.25</v>
@@ -3527,7 +3718,7 @@
     </row>
     <row r="67">
       <c r="A67" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B67" s="6">
         <v>1377.5</v>
@@ -3541,7 +3732,7 @@
     </row>
     <row r="68">
       <c r="A68" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B68" s="6">
         <v>2812</v>
@@ -3555,7 +3746,7 @@
     </row>
     <row r="69">
       <c r="A69" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B69" s="6">
         <v>1237.5</v>
@@ -3569,7 +3760,7 @@
     </row>
     <row r="70">
       <c r="A70" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B70" s="6">
         <v>8268</v>
@@ -3583,7 +3774,7 @@
     </row>
     <row r="71">
       <c r="A71" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B71" s="6">
         <v>1014</v>
@@ -3597,7 +3788,7 @@
     </row>
     <row r="72">
       <c r="A72" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B72" s="6">
         <v>740.25</v>
@@ -3611,7 +3802,7 @@
     </row>
     <row r="73">
       <c r="A73" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B73" s="6">
         <v>600.25</v>
@@ -3625,7 +3816,7 @@
     </row>
     <row r="74">
       <c r="A74" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B74" s="6">
         <v>1920</v>
@@ -3639,7 +3830,7 @@
     </row>
     <row r="75">
       <c r="A75" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B75" s="6">
         <v>328</v>
@@ -3653,7 +3844,7 @@
     </row>
     <row r="76">
       <c r="A76" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B76" s="6">
         <v>1586.5</v>
@@ -3667,7 +3858,7 @@
     </row>
     <row r="77">
       <c r="A77" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B77" s="6">
         <v>2599.26</v>
@@ -3681,7 +3872,7 @@
     </row>
     <row r="78">
       <c r="A78" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B78" s="6">
         <v>1684.75</v>
@@ -3695,7 +3886,7 @@
     </row>
     <row r="79">
       <c r="A79" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B79" s="6">
         <v>1391.75</v>
@@ -3709,7 +3900,7 @@
     </row>
     <row r="80">
       <c r="A80" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B80" s="6">
         <v>1444</v>
@@ -3723,7 +3914,7 @@
     </row>
     <row r="81">
       <c r="A81" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B81" s="6">
         <v>1368</v>
@@ -3737,7 +3928,7 @@
     </row>
     <row r="82">
       <c r="A82" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B82" s="6">
         <v>1105</v>
@@ -3751,7 +3942,7 @@
     </row>
     <row r="83">
       <c r="A83" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B83" s="6">
         <v>9997.5</v>
@@ -3765,7 +3956,7 @@
     </row>
     <row r="84">
       <c r="A84" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B84" s="6">
         <v>5637.52</v>
@@ -3779,7 +3970,7 @@
     </row>
     <row r="85">
       <c r="A85" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B85" s="6">
         <v>1930.5</v>
@@ -3793,7 +3984,7 @@
     </row>
     <row r="86">
       <c r="A86" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B86" s="6">
         <v>2600</v>
@@ -3807,7 +3998,7 @@
     </row>
     <row r="87">
       <c r="A87" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B87" s="6">
         <v>20</v>
@@ -3821,7 +4012,7 @@
     </row>
     <row r="88">
       <c r="A88" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B88" s="6">
         <v>6415.51</v>
@@ -3835,7 +4026,7 @@
     </row>
     <row r="89">
       <c r="A89" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B89" s="6">
         <v>1897.5</v>
@@ -3849,7 +4040,7 @@
     </row>
     <row r="90">
       <c r="A90" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B90" s="6">
         <v>1543.75</v>
@@ -3863,7 +4054,7 @@
     </row>
     <row r="91">
       <c r="A91" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B91" s="6">
         <v>626.5</v>
@@ -3877,7 +4068,7 @@
     </row>
     <row r="92">
       <c r="A92" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B92" s="6">
         <v>1233.75</v>
@@ -3891,7 +4082,7 @@
     </row>
     <row r="93">
       <c r="A93" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B93" s="6">
         <v>442.5</v>
@@ -3905,7 +4096,7 @@
     </row>
     <row r="94">
       <c r="A94" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B94" s="6">
         <v>2490.5</v>
@@ -3919,7 +4110,7 @@
     </row>
     <row r="95">
       <c r="A95" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B95" s="6">
         <v>3348</v>
@@ -3933,7 +4124,7 @@
     </row>
     <row r="96">
       <c r="A96" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B96" s="6">
         <v>848.25</v>
@@ -3947,7 +4138,7 @@
     </row>
     <row r="97">
       <c r="A97" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B97" s="6">
         <v>360</v>
@@ -3961,7 +4152,7 @@
     </row>
     <row r="98">
       <c r="A98" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B98" s="6">
         <v>320</v>
@@ -3975,7 +4166,7 @@
     </row>
     <row r="99">
       <c r="A99" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B99" s="6">
         <v>3060</v>
@@ -3989,7 +4180,7 @@
     </row>
     <row r="100">
       <c r="A100" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B100" s="6">
         <v>3325</v>
@@ -4003,7 +4194,7 @@
     </row>
     <row r="101">
       <c r="A101" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B101" s="6">
         <v>350</v>
@@ -4017,7 +4208,7 @@
     </row>
     <row r="102">
       <c r="A102" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B102" s="6">
         <v>2821.5</v>
@@ -4031,7 +4222,7 @@
     </row>
     <row r="103">
       <c r="A103" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B103" s="6">
         <v>3034.5</v>
@@ -4045,7 +4236,7 @@
     </row>
     <row r="104">
       <c r="A104" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B104" s="6">
         <v>365</v>
@@ -4059,7 +4250,7 @@
     </row>
     <row r="105">
       <c r="A105" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B105" s="6">
         <v>4080</v>
@@ -4073,7 +4264,7 @@
     </row>
     <row r="106">
       <c r="A106" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B106" s="6">
         <v>600</v>
@@ -4087,7 +4278,7 @@
     </row>
     <row r="107">
       <c r="A107" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B107" s="6">
         <v>648.45</v>
@@ -4101,7 +4292,7 @@
     </row>
     <row r="108">
       <c r="A108" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B108" s="6">
         <v>15504</v>
@@ -4115,7 +4306,7 @@
     </row>
     <row r="109">
       <c r="A109" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B109" s="6">
         <v>5510</v>
@@ -4129,7 +4320,7 @@
     </row>
     <row r="110">
       <c r="A110" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B110" s="6">
         <v>3377</v>
@@ -4143,7 +4334,7 @@
     </row>
     <row r="111">
       <c r="A111" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B111" s="6">
         <v>1406</v>
@@ -4157,7 +4348,7 @@
     </row>
     <row r="112">
       <c r="A112" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B112" s="6">
         <v>507.5</v>
@@ -4171,7 +4362,7 @@
     </row>
     <row r="113">
       <c r="A113" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B113" s="6">
         <v>318</v>
@@ -4185,7 +4376,7 @@
     </row>
     <row r="114">
       <c r="A114" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B114" s="6">
         <v>453</v>
@@ -4199,7 +4390,7 @@
     </row>
     <row r="115">
       <c r="A115" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B115" s="6">
         <v>660</v>
@@ -4213,7 +4404,7 @@
     </row>
     <row r="116">
       <c r="A116" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B116" s="6">
         <v>333</v>
@@ -4227,7 +4418,7 @@
     </row>
     <row r="117">
       <c r="A117" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B117" s="6">
         <v>1014</v>
@@ -4241,7 +4432,7 @@
     </row>
     <row r="118">
       <c r="A118" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B118" s="6">
         <v>1316</v>
@@ -4255,7 +4446,7 @@
     </row>
     <row r="119">
       <c r="A119" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B119" s="6">
         <v>658</v>
@@ -4269,7 +4460,7 @@
     </row>
     <row r="120">
       <c r="A120" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B120" s="6">
         <v>3633.5</v>
@@ -4283,7 +4474,7 @@
     </row>
     <row r="121">
       <c r="A121" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B121" s="6">
         <v>265.5</v>
@@ -4297,7 +4488,7 @@
     </row>
     <row r="122">
       <c r="A122" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B122" s="6">
         <v>10085.26</v>
@@ -4311,7 +4502,7 @@
     </row>
     <row r="123">
       <c r="A123" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B123" s="6">
         <v>2788</v>
@@ -4325,7 +4516,7 @@
     </row>
     <row r="124">
       <c r="A124" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B124" s="6">
         <v>410</v>
@@ -4339,7 +4530,7 @@
     </row>
     <row r="125">
       <c r="A125" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B125" s="6">
         <v>1225</v>
@@ -4353,7 +4544,7 @@
     </row>
     <row r="126">
       <c r="A126" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B126" s="6">
         <v>1264.5</v>
@@ -4367,7 +4558,7 @@
     </row>
     <row r="127">
       <c r="A127" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B127" s="6">
         <v>7947.51</v>
@@ -4381,7 +4572,7 @@
     </row>
     <row r="128">
       <c r="A128" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B128" s="6">
         <v>1334.75</v>
@@ -4395,7 +4586,7 @@
     </row>
     <row r="129">
       <c r="A129" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B129" s="6">
         <v>6884.13</v>
@@ -4409,7 +4600,7 @@
     </row>
     <row r="130">
       <c r="A130" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B130" s="6">
         <v>3969.13</v>
@@ -4423,7 +4614,7 @@
     </row>
     <row r="131">
       <c r="A131" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B131" s="6">
         <v>1444</v>
@@ -4437,7 +4628,7 @@
     </row>
     <row r="132">
       <c r="A132" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B132" s="6">
         <v>688</v>
@@ -4451,7 +4642,7 @@
     </row>
     <row r="133">
       <c r="A133" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B133" s="6">
         <v>907.5</v>
@@ -4465,7 +4656,7 @@
     </row>
     <row r="134">
       <c r="A134" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B134" s="6">
         <v>5510</v>
@@ -4479,7 +4670,7 @@
     </row>
     <row r="135">
       <c r="A135" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B135" s="6">
         <v>4981</v>
@@ -4493,7 +4684,7 @@
     </row>
     <row r="136">
       <c r="A136" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B136" s="6">
         <v>5379.38</v>
@@ -4507,7 +4698,7 @@
     </row>
     <row r="137">
       <c r="A137" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B137" s="6">
         <v>1001</v>
@@ -4521,7 +4712,7 @@
     </row>
     <row r="138">
       <c r="A138" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B138" s="6">
         <v>4812.52</v>
@@ -4535,7 +4726,7 @@
     </row>
     <row r="139">
       <c r="A139" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B139" s="6">
         <v>1287.25</v>
@@ -4549,7 +4740,7 @@
     </row>
     <row r="140">
       <c r="A140" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B140" s="6">
         <v>5946.89</v>
@@ -4563,7 +4754,7 @@
     </row>
     <row r="141">
       <c r="A141" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B141" s="6">
         <v>2431</v>
@@ -4577,7 +4768,7 @@
     </row>
     <row r="142">
       <c r="A142" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B142" s="6">
         <v>2608.5</v>
@@ -4591,7 +4782,7 @@
     </row>
     <row r="143">
       <c r="A143" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B143" s="6">
         <v>1480.5</v>
@@ -4605,7 +4796,7 @@
     </row>
     <row r="144">
       <c r="A144" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B144" s="6">
         <v>2439</v>
@@ -4619,7 +4810,7 @@
     </row>
     <row r="145">
       <c r="A145" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B145" s="6">
         <v>1642.5</v>
@@ -4633,7 +4824,7 @@
     </row>
     <row r="146">
       <c r="A146" s="0" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B146" s="6">
         <v>7172</v>
@@ -4647,7 +4838,7 @@
     </row>
     <row r="147">
       <c r="A147" s="0" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B147" s="6">
         <v>4590.63</v>
@@ -4661,7 +4852,7 @@
     </row>
     <row r="148">
       <c r="A148" s="0" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B148" s="6">
         <v>499.5</v>
@@ -4675,7 +4866,7 @@
     </row>
     <row r="149">
       <c r="A149" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B149" s="6">
         <v>3889.26</v>
@@ -4689,7 +4880,7 @@
     </row>
     <row r="150">
       <c r="A150" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B150" s="6">
         <v>783</v>
@@ -4703,7 +4894,7 @@
     </row>
     <row r="151">
       <c r="A151" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B151" s="6">
         <v>1412</v>
@@ -4717,7 +4908,7 @@
     </row>
     <row r="152">
       <c r="A152" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B152" s="6">
         <v>3278</v>
@@ -4731,7 +4922,7 @@
     </row>
     <row r="153">
       <c r="A153" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B153" s="6">
         <v>110</v>
@@ -4745,7 +4936,7 @@
     </row>
     <row r="154">
       <c r="A154" s="0" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B154" s="6">
         <v>385</v>
@@ -4759,7 +4950,7 @@
     </row>
     <row r="155">
       <c r="A155" s="0" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B155" s="6">
         <v>5310.52</v>
@@ -4773,7 +4964,7 @@
     </row>
     <row r="156">
       <c r="A156" s="0" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B156" s="6">
         <v>240</v>
@@ -4787,7 +4978,7 @@
     </row>
     <row r="157">
       <c r="A157" s="0" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B157" s="6">
         <v>535.5</v>
@@ -4801,7 +4992,7 @@
     </row>
     <row r="158">
       <c r="A158" s="0" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B158" s="6">
         <v>1539</v>
@@ -4815,7 +5006,7 @@
     </row>
     <row r="159">
       <c r="A159" s="0" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B159" s="6">
         <v>1787.5</v>
@@ -4829,7 +5020,7 @@
     </row>
     <row r="160">
       <c r="A160" s="0" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B160" s="6">
         <v>10601.51</v>
@@ -4843,7 +5034,7 @@
     </row>
     <row r="161">
       <c r="A161" s="0" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B161" s="6">
         <v>5130</v>
@@ -4857,7 +5048,7 @@
     </row>
     <row r="162">
       <c r="A162" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B162" s="6">
         <v>185</v>
@@ -4871,7 +5062,7 @@
     </row>
     <row r="163">
       <c r="A163" s="0" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B163" s="6">
         <v>3325</v>
@@ -4885,7 +5076,7 @@
     </row>
     <row r="164">
       <c r="A164" s="0" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B164" s="6">
         <v>5362.5</v>
@@ -4899,7 +5090,7 @@
     </row>
     <row r="165">
       <c r="A165" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B165" s="6">
         <v>5244</v>
@@ -4913,7 +5104,7 @@
     </row>
     <row r="166">
       <c r="A166" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B166" s="6">
         <v>2844</v>
@@ -4927,7 +5118,7 @@
     </row>
     <row r="167">
       <c r="A167" s="0" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B167" s="6">
         <v>5310.38</v>
@@ -4941,7 +5132,7 @@
     </row>
     <row r="168">
       <c r="A168" s="0" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B168" s="6">
         <v>1394.25</v>
@@ -4955,7 +5146,7 @@
     </row>
     <row r="169">
       <c r="A169" s="0" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B169" s="6">
         <v>5309.25</v>
@@ -4969,7 +5160,7 @@
     </row>
     <row r="170">
       <c r="A170" s="0" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B170" s="6">
         <v>1120</v>
@@ -4983,7 +5174,7 @@
     </row>
     <row r="171">
       <c r="A171" s="0" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B171" s="6">
         <v>2301</v>
@@ -4997,7 +5188,7 @@
     </row>
     <row r="172">
       <c r="A172" s="0" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B172" s="6">
         <v>1593</v>
@@ -5011,7 +5202,7 @@
     </row>
     <row r="173">
       <c r="A173" s="0" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B173" s="6">
         <v>885</v>
@@ -5025,7 +5216,7 @@
     </row>
     <row r="174">
       <c r="A174" s="0" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B174" s="6">
         <v>13022</v>
@@ -5039,7 +5230,7 @@
     </row>
     <row r="175">
       <c r="A175" s="0" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B175" s="6">
         <v>9369.39</v>
@@ -5053,7 +5244,7 @@
     </row>
     <row r="176">
       <c r="A176" s="0" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B176" s="6">
         <v>7012.5</v>
@@ -5067,7 +5258,7 @@
     </row>
     <row r="177">
       <c r="A177" s="0" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B177" s="6">
         <v>5293.77</v>
@@ -5081,7 +5272,7 @@
     </row>
     <row r="178">
       <c r="A178" s="0" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B178" s="6">
         <v>3387.5</v>
@@ -5095,7 +5286,7 @@
     </row>
     <row r="179">
       <c r="A179" s="0" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B179" s="6">
         <v>3184.25</v>
@@ -5109,7 +5300,7 @@
     </row>
     <row r="180">
       <c r="A180" s="0" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B180" s="6">
         <v>5843.75</v>
@@ -5123,7 +5314,7 @@
     </row>
     <row r="181">
       <c r="A181" s="0" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B181" s="6">
         <v>7493.76</v>
@@ -5137,7 +5328,7 @@
     </row>
     <row r="182">
       <c r="A182" s="0" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B182" s="6">
         <v>4878</v>
@@ -5151,7 +5342,7 @@
     </row>
     <row r="183">
       <c r="A183" s="0" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B183" s="6">
         <v>1829.26</v>
@@ -5165,7 +5356,7 @@
     </row>
     <row r="184">
       <c r="A184" s="0" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B184" s="6">
         <v>5024.26</v>
@@ -5179,7 +5370,7 @@
     </row>
     <row r="185">
       <c r="A185" s="0" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B185" s="6">
         <v>4505.88</v>
@@ -5193,7 +5384,7 @@
     </row>
     <row r="186">
       <c r="A186" s="0" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B186" s="6">
         <v>510</v>
@@ -5207,7 +5398,7 @@
     </row>
     <row r="187">
       <c r="A187" s="0" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B187" s="6">
         <v>736</v>
@@ -5221,7 +5412,7 @@
     </row>
     <row r="188">
       <c r="A188" s="0" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B188" s="6">
         <v>2520</v>
@@ -5235,7 +5426,7 @@
     </row>
     <row r="189">
       <c r="A189" s="0" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B189" s="6">
         <v>8825.01</v>
@@ -5249,7 +5440,7 @@
     </row>
     <row r="190">
       <c r="A190" s="0" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B190" s="6">
         <v>3177</v>
@@ -5263,7 +5454,7 @@
     </row>
     <row r="191">
       <c r="A191" s="0" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B191" s="6">
         <v>427.5</v>
@@ -5277,7 +5468,7 @@
     </row>
     <row r="192">
       <c r="A192" s="0" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B192" s="6">
         <v>3429.5</v>
@@ -5291,7 +5482,7 @@
     </row>
     <row r="193">
       <c r="A193" s="0" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B193" s="6">
         <v>7338.75</v>
@@ -5305,7 +5496,7 @@
     </row>
     <row r="194">
       <c r="A194" s="0" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B194" s="6">
         <v>1629.25</v>
@@ -5319,7 +5510,7 @@
     </row>
     <row r="195">
       <c r="A195" s="0" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B195" s="6">
         <v>5148</v>
@@ -5333,7 +5524,7 @@
     </row>
     <row r="196">
       <c r="A196" s="0" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B196" s="6">
         <v>202.5</v>
@@ -5347,7 +5538,7 @@
     </row>
     <row r="197">
       <c r="A197" s="0" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B197" s="6">
         <v>7475.02</v>
@@ -5361,7 +5552,7 @@
     </row>
     <row r="198">
       <c r="A198" s="0" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B198" s="6">
         <v>972</v>
@@ -5375,7 +5566,7 @@
     </row>
     <row r="199">
       <c r="A199" s="0" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B199" s="6">
         <v>11680</v>
@@ -5389,7 +5580,7 @@
     </row>
     <row r="200">
       <c r="A200" s="0" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B200" s="6">
         <v>2992</v>
@@ -5403,7 +5594,7 @@
     </row>
     <row r="201">
       <c r="A201" s="0" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B201" s="6">
         <v>8370.63</v>
@@ -5417,7 +5608,7 @@
     </row>
     <row r="202">
       <c r="A202" s="0" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B202" s="6">
         <v>1567.5</v>
@@ -5431,7 +5622,7 @@
     </row>
     <row r="203">
       <c r="A203" s="0" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B203" s="6">
         <v>1106</v>
@@ -5445,7 +5636,7 @@
     </row>
     <row r="204">
       <c r="A204" s="0" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B204" s="6">
         <v>2472</v>
@@ -5459,7 +5650,7 @@
     </row>
     <row r="205">
       <c r="A205" s="0" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B205" s="6">
         <v>2450.5</v>
@@ -5473,7 +5664,7 @@
     </row>
     <row r="206">
       <c r="A206" s="0" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B206" s="6">
         <v>1560</v>
@@ -5487,7 +5678,7 @@
     </row>
     <row r="207">
       <c r="A207" s="0" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B207" s="6">
         <v>490.5</v>
@@ -5501,7 +5692,7 @@
     </row>
     <row r="208">
       <c r="A208" s="0" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B208" s="6">
         <v>16159</v>
@@ -5515,7 +5706,7 @@
     </row>
     <row r="209">
       <c r="A209" s="0" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B209" s="6">
         <v>4119.63</v>
@@ -5529,7 +5720,7 @@
     </row>
     <row r="210">
       <c r="A210" s="0" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="B210" s="6">
         <v>17004</v>
@@ -5543,7 +5734,7 @@
     </row>
     <row r="211">
       <c r="A211" s="0" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B211" s="6">
         <v>4230</v>
@@ -5557,7 +5748,7 @@
     </row>
     <row r="212">
       <c r="A212" s="0" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B212" s="6">
         <v>2860</v>
@@ -5571,7 +5762,7 @@
     </row>
     <row r="213">
       <c r="A213" s="0" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B213" s="6">
         <v>5740.63</v>
@@ -5585,7 +5776,7 @@
     </row>
     <row r="214">
       <c r="A214" s="0" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B214" s="6">
         <v>1548.5</v>
@@ -5599,7 +5790,7 @@
     </row>
     <row r="215">
       <c r="A215" s="0" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B215" s="6">
         <v>652</v>
@@ -5613,7 +5804,7 @@
     </row>
     <row r="216">
       <c r="A216" s="0" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B216" s="6">
         <v>9685</v>
@@ -5627,7 +5818,7 @@
     </row>
     <row r="217">
       <c r="A217" s="0" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B217" s="6">
         <v>1608.75</v>
@@ -5641,7 +5832,7 @@
     </row>
     <row r="218">
       <c r="A218" s="0" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B218" s="6">
         <v>990</v>
@@ -5655,7 +5846,7 @@
     </row>
     <row r="219">
       <c r="A219" s="0" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B219" s="6">
         <v>328</v>
@@ -5669,7 +5860,7 @@
     </row>
     <row r="220">
       <c r="A220" s="0" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B220" s="6">
         <v>504</v>
@@ -5683,7 +5874,7 @@
     </row>
     <row r="221">
       <c r="A221" s="0" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="B221" s="6">
         <v>960</v>
@@ -5697,7 +5888,7 @@
     </row>
     <row r="222">
       <c r="A222" s="0" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B222" s="6">
         <v>5492.38</v>
@@ -5711,7 +5902,7 @@
     </row>
     <row r="223">
       <c r="A223" s="0" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B223" s="6">
         <v>7567</v>
@@ -5725,7 +5916,7 @@
     </row>
     <row r="224">
       <c r="A224" s="0" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B224" s="6">
         <v>1684.38</v>
@@ -5739,7 +5930,7 @@
     </row>
     <row r="225">
       <c r="A225" s="0" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B225" s="6">
         <v>1358.5</v>
@@ -5753,7 +5944,7 @@
     </row>
     <row r="226">
       <c r="A226" s="0" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B226" s="6">
         <v>15768</v>
@@ -5767,7 +5958,7 @@
     </row>
     <row r="227">
       <c r="A227" s="0" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B227" s="6">
         <v>2231.25</v>
@@ -5781,7 +5972,7 @@
     </row>
     <row r="228">
       <c r="A228" s="0" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B228" s="6">
         <v>370</v>
@@ -5795,7 +5986,7 @@
     </row>
     <row r="229">
       <c r="A229" s="0" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B229" s="6">
         <v>1008</v>
@@ -5809,7 +6000,7 @@
     </row>
     <row r="230">
       <c r="A230" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B230" s="6">
         <v>11304</v>
@@ -5823,7 +6014,7 @@
     </row>
     <row r="231">
       <c r="A231" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="B231" s="6">
         <v>3116</v>
@@ -5837,7 +6028,7 @@
     </row>
     <row r="232">
       <c r="A232" s="0" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B232" s="6">
         <v>2335.5</v>
@@ -5851,7 +6042,7 @@
     </row>
     <row r="233">
       <c r="A233" s="0" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B233" s="6">
         <v>2756.25</v>
@@ -5865,7 +6056,7 @@
     </row>
     <row r="234">
       <c r="A234" s="0" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B234" s="6">
         <v>1197</v>
@@ -5879,7 +6070,7 @@
     </row>
     <row r="235">
       <c r="A235" s="0" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B235" s="6">
         <v>3146</v>
@@ -5893,7 +6084,7 @@
     </row>
     <row r="236">
       <c r="A236" s="0" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B236" s="6">
         <v>7053.75</v>
@@ -5907,7 +6098,7 @@
     </row>
     <row r="237">
       <c r="A237" s="0" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B237" s="6">
         <v>510</v>
@@ -5921,7 +6112,7 @@
     </row>
     <row r="238">
       <c r="A238" s="0" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B238" s="6">
         <v>716</v>
@@ -5935,7 +6126,7 @@
     </row>
     <row r="239">
       <c r="A239" s="0" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B239" s="6">
         <v>4047</v>
@@ -5949,7 +6140,7 @@
     </row>
     <row r="240">
       <c r="A240" s="0" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="B240" s="6">
         <v>10792</v>
@@ -5963,7 +6154,7 @@
     </row>
     <row r="241">
       <c r="A241" s="0" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B241" s="6">
         <v>340</v>
@@ -5977,7 +6168,7 @@
     </row>
     <row r="242">
       <c r="A242" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="B242" s="6">
         <v>680</v>
@@ -5991,7 +6182,7 @@
     </row>
     <row r="243">
       <c r="A243" s="0" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="B243" s="6">
         <v>2649</v>
@@ -6005,7 +6196,7 @@
     </row>
     <row r="244">
       <c r="A244" s="0" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="B244" s="6">
         <v>1656</v>
@@ -6019,7 +6210,7 @@
     </row>
     <row r="245">
       <c r="A245" s="0" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="B245" s="6">
         <v>1007.5</v>
@@ -6033,7 +6224,7 @@
     </row>
     <row r="246">
       <c r="A246" s="0" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B246" s="6">
         <v>1306.25</v>
@@ -6047,7 +6238,7 @@
     </row>
     <row r="247">
       <c r="A247" s="0" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B247" s="6">
         <v>2909.5</v>
@@ -6061,7 +6252,7 @@
     </row>
     <row r="248">
       <c r="A248" s="0" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="B248" s="6">
         <v>4778.13</v>
@@ -6075,7 +6266,7 @@
     </row>
     <row r="249">
       <c r="A249" s="0" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B249" s="6">
         <v>2193.13</v>
@@ -6089,7 +6280,7 @@
     </row>
     <row r="250">
       <c r="A250" s="0" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="B250" s="6">
         <v>351</v>
@@ -6103,7 +6294,7 @@
     </row>
     <row r="251">
       <c r="A251" s="0" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="B251" s="6">
         <v>1620</v>
@@ -6117,7 +6308,7 @@
     </row>
     <row r="252">
       <c r="A252" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B252" s="6">
         <v>6707</v>
@@ -6131,7 +6322,7 @@
     </row>
     <row r="253">
       <c r="A253" s="0" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B253" s="6">
         <v>360</v>
@@ -6145,7 +6336,7 @@
     </row>
     <row r="254">
       <c r="A254" s="0" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B254" s="6">
         <v>240</v>
@@ -6159,7 +6350,7 @@
     </row>
     <row r="255">
       <c r="A255" s="0" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B255" s="6">
         <v>3267.01</v>
@@ -6173,7 +6364,7 @@
     </row>
     <row r="256">
       <c r="A256" s="0" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="B256" s="6">
         <v>4617</v>
@@ -6187,7 +6378,7 @@
     </row>
     <row r="257">
       <c r="A257" s="0" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="B257" s="6">
         <v>716</v>
@@ -6201,7 +6392,7 @@
     </row>
     <row r="258">
       <c r="A258" s="0" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B258" s="6">
         <v>3078</v>
@@ -6215,7 +6406,7 @@
     </row>
     <row r="259">
       <c r="A259" s="0" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="B259" s="6">
         <v>1472</v>
@@ -6229,7 +6420,7 @@
     </row>
     <row r="260">
       <c r="A260" s="0" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="B260" s="6">
         <v>389.25</v>
@@ -6243,7 +6434,7 @@
     </row>
     <row r="261">
       <c r="A261" s="0" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="B261" s="6">
         <v>4635</v>
@@ -6257,7 +6448,7 @@
     </row>
     <row r="262">
       <c r="A262" s="0" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="B262" s="6">
         <v>4864</v>
@@ -6271,7 +6462,7 @@
     </row>
     <row r="263">
       <c r="A263" s="0" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="B263" s="6">
         <v>1444</v>
@@ -6285,7 +6476,7 @@
     </row>
     <row r="264">
       <c r="A264" s="0" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="B264" s="6">
         <v>708</v>
@@ -6299,7 +6490,7 @@
     </row>
     <row r="265">
       <c r="A265" s="0" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="B265" s="6">
         <v>2064</v>
@@ -6313,7 +6504,7 @@
     </row>
     <row r="266">
       <c r="A266" s="0" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B266" s="6">
         <v>368</v>
@@ -6327,7 +6518,7 @@
     </row>
     <row r="267">
       <c r="A267" s="0" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="B267" s="6">
         <v>187.5</v>
@@ -6341,7 +6532,7 @@
     </row>
     <row r="268">
       <c r="A268" s="0" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="B268" s="6">
         <v>12780</v>
@@ -6355,7 +6546,7 @@
     </row>
     <row r="269">
       <c r="A269" s="0" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="B269" s="6">
         <v>3262</v>
@@ -6369,7 +6560,7 @@
     </row>
     <row r="270">
       <c r="A270" s="0" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B270" s="6">
         <v>1440</v>
@@ -6383,7 +6574,7 @@
     </row>
     <row r="271">
       <c r="A271" s="0" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="B271" s="6">
         <v>5505.25</v>
@@ -6397,7 +6588,7 @@
     </row>
     <row r="272">
       <c r="A272" s="0" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="B272" s="6">
         <v>756</v>
@@ -6411,7 +6602,7 @@
     </row>
     <row r="273">
       <c r="A273" s="0" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="B273" s="6">
         <v>181.5</v>
@@ -6425,7 +6616,7 @@
     </row>
     <row r="274">
       <c r="A274" s="0" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="B274" s="6">
         <v>514.5</v>
@@ -6439,7 +6630,7 @@
     </row>
     <row r="275">
       <c r="A275" s="0" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="B275" s="6">
         <v>3078</v>
@@ -6453,7 +6644,7 @@
     </row>
     <row r="276">
       <c r="A276" s="0" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="B276" s="6">
         <v>178.5</v>
@@ -6467,7 +6658,7 @@
     </row>
     <row r="277">
       <c r="A277" s="0" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="B277" s="6">
         <v>306</v>
@@ -6481,7 +6672,7 @@
     </row>
     <row r="278">
       <c r="A278" s="0" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="B278" s="6">
         <v>1377.5</v>
@@ -6495,7 +6686,7 @@
     </row>
     <row r="279">
       <c r="A279" s="0" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="B279" s="6">
         <v>428.75</v>
@@ -6509,7 +6700,7 @@
     </row>
     <row r="280">
       <c r="A280" s="0" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B280" s="6">
         <v>1020</v>
@@ -6523,7 +6714,7 @@
     </row>
     <row r="281">
       <c r="A281" s="0" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="B281" s="6">
         <v>1440</v>
@@ -6537,7 +6728,7 @@
     </row>
     <row r="282">
       <c r="A282" s="0" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="B282" s="6">
         <v>1593</v>
@@ -6551,7 +6742,7 @@
     </row>
     <row r="283">
       <c r="A283" s="0" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="B283" s="6">
         <v>1714.75</v>
@@ -6565,7 +6756,7 @@
     </row>
     <row r="284">
       <c r="A284" s="0" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B284" s="6">
         <v>1358.5</v>
@@ -6579,7 +6770,7 @@
     </row>
     <row r="285">
       <c r="A285" s="0" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="B285" s="6">
         <v>606.13</v>
@@ -6593,7 +6784,7 @@
     </row>
     <row r="286">
       <c r="A286" s="0" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="B286" s="6">
         <v>852.5</v>
@@ -6607,7 +6798,7 @@
     </row>
     <row r="287">
       <c r="A287" s="0" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="B287" s="6">
         <v>11232</v>
@@ -6621,7 +6812,7 @@
     </row>
     <row r="288">
       <c r="A288" s="0" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="B288" s="6">
         <v>825</v>
@@ -6635,7 +6826,7 @@
     </row>
     <row r="289">
       <c r="A289" s="0" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="B289" s="6">
         <v>4716.25</v>
@@ -6649,7 +6840,7 @@
     </row>
     <row r="290">
       <c r="A290" s="0" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="B290" s="6">
         <v>2698</v>
@@ -6663,7 +6854,7 @@
     </row>
     <row r="291">
       <c r="A291" s="0" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B291" s="6">
         <v>3755.5</v>
@@ -6677,7 +6868,7 @@
     </row>
     <row r="292">
       <c r="A292" s="0" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B292" s="6">
         <v>7317</v>
@@ -6691,7 +6882,7 @@
     </row>
     <row r="293">
       <c r="A293" s="0" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B293" s="6">
         <v>1980</v>
@@ -6705,7 +6896,7 @@
     </row>
     <row r="294">
       <c r="A294" s="0" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="B294" s="6">
         <v>4873.5</v>
@@ -6719,7 +6910,7 @@
     </row>
     <row r="295">
       <c r="A295" s="0" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="B295" s="6">
         <v>1790</v>
@@ -6733,7 +6924,7 @@
     </row>
     <row r="296">
       <c r="A296" s="0" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="B296" s="6">
         <v>1134</v>
@@ -6747,7 +6938,7 @@
     </row>
     <row r="297">
       <c r="A297" s="0" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="B297" s="6">
         <v>1358.5</v>
@@ -6761,7 +6952,7 @@
     </row>
     <row r="298">
       <c r="A298" s="0" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="B298" s="6">
         <v>7678.13</v>
@@ -6775,7 +6966,7 @@
     </row>
     <row r="299">
       <c r="A299" s="0" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="B299" s="6">
         <v>1335</v>
@@ -6789,7 +6980,7 @@
     </row>
     <row r="300">
       <c r="A300" s="0" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="B300" s="6">
         <v>660</v>
@@ -6803,7 +6994,7 @@
     </row>
     <row r="301">
       <c r="A301" s="0" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B301" s="6">
         <v>328</v>
@@ -6817,7 +7008,7 @@
     </row>
     <row r="302">
       <c r="A302" s="0" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="B302" s="6">
         <v>6581.25</v>
@@ -6831,7 +7022,7 @@
     </row>
     <row r="303">
       <c r="A303" s="0" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="B303" s="6">
         <v>6320</v>
@@ -6845,7 +7036,7 @@
     </row>
     <row r="304">
       <c r="A304" s="0" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="B304" s="6">
         <v>574</v>
@@ -6859,7 +7050,7 @@
     </row>
     <row r="305">
       <c r="A305" s="0" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="B305" s="6">
         <v>1200</v>
@@ -6873,7 +7064,7 @@
     </row>
     <row r="306">
       <c r="A306" s="0" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="B306" s="6">
         <v>5492.38</v>
@@ -6887,7 +7078,7 @@
     </row>
     <row r="307">
       <c r="A307" s="0" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="B307" s="6">
         <v>3826.63</v>
@@ -6901,7 +7092,7 @@
     </row>
     <row r="308">
       <c r="A308" s="0" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="B308" s="6">
         <v>5415</v>
@@ -6915,7 +7106,7 @@
     </row>
     <row r="309">
       <c r="A309" s="0" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="B309" s="6">
         <v>3003</v>
@@ -6929,7 +7120,7 @@
     </row>
     <row r="310">
       <c r="A310" s="0" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="B310" s="6">
         <v>4800</v>
@@ -6943,7 +7134,7 @@
     </row>
     <row r="311">
       <c r="A311" s="0" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B311" s="6">
         <v>2831</v>
@@ -6957,7 +7148,7 @@
     </row>
     <row r="312">
       <c r="A312" s="0" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B312" s="6">
         <v>6006</v>
@@ -6971,7 +7162,7 @@
     </row>
     <row r="313">
       <c r="A313" s="0" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B313" s="6">
         <v>1505.16</v>
@@ -6985,7 +7176,7 @@
     </row>
     <row r="314">
       <c r="A314" s="0" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="B314" s="6">
         <v>99</v>
@@ -6999,7 +7190,7 @@
     </row>
     <row r="315">
       <c r="A315" s="0" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="B315" s="6">
         <v>3543.5</v>
@@ -7013,7 +7204,7 @@
     </row>
     <row r="316">
       <c r="A316" s="0" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B316" s="6">
         <v>1452</v>
@@ -7027,7 +7218,7 @@
     </row>
     <row r="317">
       <c r="A317" s="0" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="B317" s="6">
         <v>358</v>
@@ -7041,7 +7232,7 @@
     </row>
     <row r="318">
       <c r="A318" s="0" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="B318" s="6">
         <v>4332</v>
@@ -7055,7 +7246,7 @@
     </row>
     <row r="319">
       <c r="A319" s="0" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="B319" s="6">
         <v>1695.75</v>
@@ -7069,7 +7260,7 @@
     </row>
     <row r="320">
       <c r="A320" s="0" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B320" s="6">
         <v>6906.25</v>
@@ -7083,7 +7274,7 @@
     </row>
     <row r="321">
       <c r="A321" s="0" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B321" s="6">
         <v>552</v>
@@ -7097,7 +7288,7 @@
     </row>
     <row r="322">
       <c r="A322" s="0" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B322" s="6">
         <v>5130</v>
@@ -7111,7 +7302,7 @@
     </row>
     <row r="323">
       <c r="A323" s="0" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="B323" s="6">
         <v>4323</v>
@@ -7125,7 +7316,7 @@
     </row>
     <row r="324">
       <c r="A324" s="0" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="B324" s="6">
         <v>182</v>
@@ -7139,7 +7330,7 @@
     </row>
     <row r="325">
       <c r="A325" s="0" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="B325" s="6">
         <v>1835</v>
@@ -7153,7 +7344,7 @@
     </row>
     <row r="326">
       <c r="A326" s="0" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="B326" s="6">
         <v>775</v>
@@ -7167,7 +7358,7 @@
     </row>
     <row r="327">
       <c r="A327" s="0" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="B327" s="6">
         <v>343</v>
@@ -7181,7 +7372,7 @@
     </row>
     <row r="328">
       <c r="A328" s="0" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="B328" s="6">
         <v>2087.5</v>
@@ -7195,7 +7386,7 @@
     </row>
     <row r="329">
       <c r="A329" s="0" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="B329" s="6">
         <v>17242.5</v>
@@ -7209,7 +7400,7 @@
     </row>
     <row r="330">
       <c r="A330" s="0" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="B330" s="6">
         <v>7128</v>
@@ -7223,7 +7414,7 @@
     </row>
     <row r="331">
       <c r="A331" s="0" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="B331" s="6">
         <v>6127.5</v>
@@ -7237,7 +7428,7 @@
     </row>
     <row r="332">
       <c r="A332" s="0" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="B332" s="6">
         <v>1620</v>
@@ -7251,7 +7442,7 @@
     </row>
     <row r="333">
       <c r="A333" s="0" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="B333" s="6">
         <v>10656.26</v>
@@ -7265,7 +7456,7 @@
     </row>
     <row r="334">
       <c r="A334" s="0" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="B334" s="6">
         <v>27702</v>
@@ -7279,7 +7470,7 @@
     </row>
     <row r="335">
       <c r="A335" s="0" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="B335" s="6">
         <v>2112.5</v>
@@ -7293,7 +7484,7 @@
     </row>
     <row r="336">
       <c r="A336" s="0" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="B336" s="6">
         <v>37100</v>
@@ -7307,7 +7498,7 @@
     </row>
     <row r="337">
       <c r="A337" s="0" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="B337" s="6">
         <v>8381.25</v>
@@ -7321,7 +7512,7 @@
     </row>
     <row r="338">
       <c r="A338" s="0" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="B338" s="6">
         <v>3259.63</v>
@@ -7335,7 +7526,7 @@
     </row>
     <row r="339">
       <c r="A339" s="0" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="B339" s="6">
         <v>14085.5</v>
@@ -7349,7 +7540,7 @@
     </row>
     <row r="340">
       <c r="A340" s="0" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="B340" s="6">
         <v>4189.5</v>
@@ -7363,7 +7554,7 @@
     </row>
     <row r="341">
       <c r="A341" s="0" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="B341" s="6">
         <v>4171.5</v>
@@ -7377,7 +7568,7 @@
     </row>
     <row r="342">
       <c r="A342" s="0" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="B342" s="6">
         <v>50</v>
@@ -7391,7 +7582,7 @@
     </row>
     <row r="343">
       <c r="A343" s="0" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="B343" s="6">
         <v>316.5</v>
@@ -7405,7 +7596,7 @@
     </row>
     <row r="344">
       <c r="A344" s="0" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="B344" s="6">
         <v>484.5</v>

</xml_diff>

<commit_message>
Sync GTD brain 2026-02-18
</commit_message>
<xml_diff>
--- a/Projects/tbh-report-catalog/reports/202501 DispatchBilling Verification Pack.xlsx
+++ b/Projects/tbh-report-catalog/reports/202501 DispatchBilling Verification Pack.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="758" uniqueCount="758">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="764" uniqueCount="764">
   <si>
     <t>TBH Dispatch / Billing Verification Pack</t>
   </si>
@@ -29,7 +29,7 @@
     <t>Generated</t>
   </si>
   <si>
-    <t>2026-02-17 17:44</t>
+    <t>2026-02-18 09:43</t>
   </si>
   <si>
     <t>Notes</t>
@@ -2289,6 +2289,24 @@
   </si>
   <si>
     <t>1483548</t>
+  </si>
+  <si>
+    <t>1483667</t>
+  </si>
+  <si>
+    <t>1483668</t>
+  </si>
+  <si>
+    <t>1484728</t>
+  </si>
+  <si>
+    <t>1484729</t>
+  </si>
+  <si>
+    <t>1484730</t>
+  </si>
+  <si>
+    <t>1484731</t>
   </si>
 </sst>
 </file>
@@ -2488,7 +2506,7 @@
         <v>19</v>
       </c>
       <c r="D3" s="5">
-        <v>99.5</v>
+        <v>0</v>
       </c>
       <c r="E3" s="6">
         <v>15109.51</v>
@@ -2511,7 +2529,7 @@
         <v>21</v>
       </c>
       <c r="D4" s="5">
-        <v>71.5</v>
+        <v>0</v>
       </c>
       <c r="E4" s="6">
         <v>11158.5</v>
@@ -2534,7 +2552,7 @@
         <v>23</v>
       </c>
       <c r="D5" s="5">
-        <v>198.75</v>
+        <v>0</v>
       </c>
       <c r="E5" s="6">
         <v>30699.01</v>
@@ -2580,7 +2598,7 @@
         <v>25</v>
       </c>
       <c r="D7" s="5">
-        <v>235</v>
+        <v>0</v>
       </c>
       <c r="E7" s="6">
         <v>35391.27</v>
@@ -2603,7 +2621,7 @@
         <v>19</v>
       </c>
       <c r="D8" s="5">
-        <v>116</v>
+        <v>0</v>
       </c>
       <c r="E8" s="6">
         <v>18037.77</v>
@@ -2626,7 +2644,7 @@
         <v>21</v>
       </c>
       <c r="D9" s="5">
-        <v>183.25</v>
+        <v>0</v>
       </c>
       <c r="E9" s="6">
         <v>27815.75</v>
@@ -2649,7 +2667,7 @@
         <v>23</v>
       </c>
       <c r="D10" s="5">
-        <v>425.5</v>
+        <v>0</v>
       </c>
       <c r="E10" s="6">
         <v>66194.56</v>
@@ -2741,7 +2759,7 @@
         <v>25</v>
       </c>
       <c r="D14" s="5">
-        <v>409.25</v>
+        <v>0</v>
       </c>
       <c r="E14" s="6">
         <v>60660.9</v>
@@ -2764,7 +2782,7 @@
         <v>23</v>
       </c>
       <c r="D15" s="5">
-        <v>47</v>
+        <v>0</v>
       </c>
       <c r="E15" s="6">
         <v>10601.51</v>
@@ -2787,7 +2805,7 @@
         <v>19</v>
       </c>
       <c r="D16" s="5">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E16" s="6">
         <v>1647</v>
@@ -2810,7 +2828,7 @@
         <v>21</v>
       </c>
       <c r="D17" s="5">
-        <v>44</v>
+        <v>0</v>
       </c>
       <c r="E17" s="6">
         <v>7264</v>
@@ -2833,7 +2851,7 @@
         <v>25</v>
       </c>
       <c r="D18" s="5">
-        <v>39</v>
+        <v>0</v>
       </c>
       <c r="E18" s="6">
         <v>6957.5</v>
@@ -2856,7 +2874,7 @@
         <v>19</v>
       </c>
       <c r="D19" s="5">
-        <v>45.5</v>
+        <v>0</v>
       </c>
       <c r="E19" s="6">
         <v>7837</v>
@@ -2879,7 +2897,7 @@
         <v>21</v>
       </c>
       <c r="D20" s="5">
-        <v>102</v>
+        <v>0</v>
       </c>
       <c r="E20" s="6">
         <v>15643</v>
@@ -2902,7 +2920,7 @@
         <v>23</v>
       </c>
       <c r="D21" s="5">
-        <v>109</v>
+        <v>0</v>
       </c>
       <c r="E21" s="6">
         <v>16074.5</v>
@@ -2948,7 +2966,7 @@
         <v>25</v>
       </c>
       <c r="D23" s="5">
-        <v>75</v>
+        <v>0</v>
       </c>
       <c r="E23" s="6">
         <v>12519</v>
@@ -2971,7 +2989,7 @@
         <v>19</v>
       </c>
       <c r="D24" s="5">
-        <v>105</v>
+        <v>0</v>
       </c>
       <c r="E24" s="6">
         <v>16723.27</v>
@@ -2994,7 +3012,7 @@
         <v>21</v>
       </c>
       <c r="D25" s="5">
-        <v>226</v>
+        <v>0</v>
       </c>
       <c r="E25" s="6">
         <v>32755.52</v>
@@ -3017,7 +3035,7 @@
         <v>23</v>
       </c>
       <c r="D26" s="5">
-        <v>352.75</v>
+        <v>0</v>
       </c>
       <c r="E26" s="6">
         <v>53269.53</v>
@@ -3040,7 +3058,7 @@
         <v>25</v>
       </c>
       <c r="D27" s="5">
-        <v>325.75</v>
+        <v>0</v>
       </c>
       <c r="E27" s="6">
         <v>50489.91</v>
@@ -3063,7 +3081,7 @@
         <v>19</v>
       </c>
       <c r="D28" s="5">
-        <v>112.5</v>
+        <v>0</v>
       </c>
       <c r="E28" s="6">
         <v>18138.25</v>
@@ -3086,7 +3104,7 @@
         <v>21</v>
       </c>
       <c r="D29" s="5">
-        <v>414.75</v>
+        <v>0</v>
       </c>
       <c r="E29" s="6">
         <v>60074.13</v>
@@ -3109,7 +3127,7 @@
         <v>23</v>
       </c>
       <c r="D30" s="5">
-        <v>657.25</v>
+        <v>0</v>
       </c>
       <c r="E30" s="6">
         <v>98735.64</v>
@@ -3155,7 +3173,7 @@
         <v>25</v>
       </c>
       <c r="D32" s="5">
-        <v>282</v>
+        <v>0</v>
       </c>
       <c r="E32" s="6">
         <v>42290.75</v>
@@ -3178,7 +3196,7 @@
         <v>19</v>
       </c>
       <c r="D33" s="5">
-        <v>54.5</v>
+        <v>0</v>
       </c>
       <c r="E33" s="6">
         <v>8279.75</v>
@@ -3201,7 +3219,7 @@
         <v>21</v>
       </c>
       <c r="D34" s="5">
-        <v>110.5</v>
+        <v>0</v>
       </c>
       <c r="E34" s="6">
         <v>15859</v>
@@ -3224,7 +3242,7 @@
         <v>23</v>
       </c>
       <c r="D35" s="5">
-        <v>123.5</v>
+        <v>0</v>
       </c>
       <c r="E35" s="6">
         <v>18884.26</v>
@@ -3270,7 +3288,7 @@
         <v>25</v>
       </c>
       <c r="D37" s="5">
-        <v>159</v>
+        <v>0</v>
       </c>
       <c r="E37" s="6">
         <v>25177.51</v>
@@ -3293,7 +3311,7 @@
         <v>19</v>
       </c>
       <c r="D38" s="5">
-        <v>111.25</v>
+        <v>0</v>
       </c>
       <c r="E38" s="6">
         <v>18174.26</v>
@@ -3316,7 +3334,7 @@
         <v>21</v>
       </c>
       <c r="D39" s="5">
-        <v>51.5</v>
+        <v>0</v>
       </c>
       <c r="E39" s="6">
         <v>7016</v>
@@ -3339,7 +3357,7 @@
         <v>23</v>
       </c>
       <c r="D40" s="5">
-        <v>280.75</v>
+        <v>0</v>
       </c>
       <c r="E40" s="6">
         <v>43232</v>
@@ -3408,7 +3426,7 @@
         <v>25</v>
       </c>
       <c r="D43" s="5">
-        <v>155.5</v>
+        <v>0</v>
       </c>
       <c r="E43" s="6">
         <v>25606.75</v>
@@ -3431,7 +3449,7 @@
         <v>19</v>
       </c>
       <c r="D44" s="5">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="E44" s="6">
         <v>3952.5</v>
@@ -3454,7 +3472,7 @@
         <v>21</v>
       </c>
       <c r="D45" s="5">
-        <v>46.5</v>
+        <v>0</v>
       </c>
       <c r="E45" s="6">
         <v>7880</v>
@@ -3477,7 +3495,7 @@
         <v>23</v>
       </c>
       <c r="D46" s="5">
-        <v>316</v>
+        <v>0</v>
       </c>
       <c r="E46" s="6">
         <v>48372.26</v>
@@ -3523,7 +3541,7 @@
         <v>25</v>
       </c>
       <c r="D48" s="5">
-        <v>334</v>
+        <v>0</v>
       </c>
       <c r="E48" s="6">
         <v>52175.01</v>
@@ -3546,7 +3564,7 @@
         <v>19</v>
       </c>
       <c r="D49" s="5">
-        <v>242.5</v>
+        <v>0</v>
       </c>
       <c r="E49" s="6">
         <v>39535.28</v>
@@ -3569,7 +3587,7 @@
         <v>21</v>
       </c>
       <c r="D50" s="5">
-        <v>355</v>
+        <v>0</v>
       </c>
       <c r="E50" s="6">
         <v>57749.63</v>
@@ -3592,7 +3610,7 @@
         <v>23</v>
       </c>
       <c r="D51" s="5">
-        <v>1161.25</v>
+        <v>0</v>
       </c>
       <c r="E51" s="6">
         <v>170265.41</v>
@@ -3661,7 +3679,7 @@
         <v>25</v>
       </c>
       <c r="D54" s="5">
-        <v>595.75</v>
+        <v>0</v>
       </c>
       <c r="E54" s="6">
         <v>95708.39</v>
@@ -3730,7 +3748,7 @@
         <v>23</v>
       </c>
       <c r="D57" s="5">
-        <v>106.75</v>
+        <v>0</v>
       </c>
       <c r="E57" s="6">
         <v>16521.5</v>
@@ -3776,7 +3794,7 @@
         <v>25</v>
       </c>
       <c r="D59" s="5">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="E59" s="6">
         <v>13371.5</v>
@@ -3799,7 +3817,7 @@
         <v>19</v>
       </c>
       <c r="D60" s="5">
-        <v>110.75</v>
+        <v>0</v>
       </c>
       <c r="E60" s="6">
         <v>17618.9</v>
@@ -3822,7 +3840,7 @@
         <v>21</v>
       </c>
       <c r="D61" s="5">
-        <v>205.5</v>
+        <v>0</v>
       </c>
       <c r="E61" s="6">
         <v>29863.53</v>
@@ -3845,7 +3863,7 @@
         <v>23</v>
       </c>
       <c r="D62" s="5">
-        <v>191.5</v>
+        <v>0</v>
       </c>
       <c r="E62" s="6">
         <v>28785.5</v>
@@ -3891,7 +3909,7 @@
         <v>25</v>
       </c>
       <c r="D64" s="5">
-        <v>187.5</v>
+        <v>0</v>
       </c>
       <c r="E64" s="6">
         <v>27854.52</v>
@@ -3914,7 +3932,7 @@
         <v>19</v>
       </c>
       <c r="D65" s="5">
-        <v>81</v>
+        <v>0</v>
       </c>
       <c r="E65" s="6">
         <v>13116</v>
@@ -3937,7 +3955,7 @@
         <v>21</v>
       </c>
       <c r="D66" s="5">
-        <v>144.5</v>
+        <v>0</v>
       </c>
       <c r="E66" s="6">
         <v>22872</v>
@@ -3960,7 +3978,7 @@
         <v>23</v>
       </c>
       <c r="D67" s="5">
-        <v>748</v>
+        <v>0</v>
       </c>
       <c r="E67" s="6">
         <v>111639.93</v>
@@ -4029,7 +4047,7 @@
         <v>25</v>
       </c>
       <c r="D70" s="5">
-        <v>197.75</v>
+        <v>0</v>
       </c>
       <c r="E70" s="6">
         <v>28558.78</v>
@@ -4052,7 +4070,7 @@
         <v>19</v>
       </c>
       <c r="D71" s="5">
-        <v>49</v>
+        <v>0</v>
       </c>
       <c r="E71" s="6">
         <v>8748.5</v>
@@ -4075,7 +4093,7 @@
         <v>21</v>
       </c>
       <c r="D72" s="5">
-        <v>126.5</v>
+        <v>0</v>
       </c>
       <c r="E72" s="6">
         <v>19559.75</v>
@@ -4098,7 +4116,7 @@
         <v>23</v>
       </c>
       <c r="D73" s="5">
-        <v>546.75</v>
+        <v>0</v>
       </c>
       <c r="E73" s="6">
         <v>81670.4</v>
@@ -4167,7 +4185,7 @@
         <v>25</v>
       </c>
       <c r="D76" s="5">
-        <v>368.5</v>
+        <v>0</v>
       </c>
       <c r="E76" s="6">
         <v>58499.13</v>
@@ -4190,7 +4208,7 @@
         <v>19</v>
       </c>
       <c r="D77" s="5">
-        <v>110.5</v>
+        <v>0</v>
       </c>
       <c r="E77" s="6">
         <v>20473.38</v>
@@ -4213,7 +4231,7 @@
         <v>21</v>
       </c>
       <c r="D78" s="5">
-        <v>413.5</v>
+        <v>0</v>
       </c>
       <c r="E78" s="6">
         <v>60455</v>
@@ -4236,7 +4254,7 @@
         <v>23</v>
       </c>
       <c r="D79" s="5">
-        <v>722.75</v>
+        <v>0</v>
       </c>
       <c r="E79" s="6">
         <v>111327.65</v>
@@ -4259,7 +4277,7 @@
         <v>25</v>
       </c>
       <c r="D80" s="5">
-        <v>297.75</v>
+        <v>0</v>
       </c>
       <c r="E80" s="6">
         <v>44888.38</v>
@@ -4282,7 +4300,7 @@
         <v>19</v>
       </c>
       <c r="D81" s="5">
-        <v>173</v>
+        <v>0</v>
       </c>
       <c r="E81" s="6">
         <v>28148</v>
@@ -4305,7 +4323,7 @@
         <v>21</v>
       </c>
       <c r="D82" s="5">
-        <v>315.25</v>
+        <v>0</v>
       </c>
       <c r="E82" s="6">
         <v>44434.5</v>
@@ -4328,7 +4346,7 @@
         <v>23</v>
       </c>
       <c r="D83" s="5">
-        <v>928</v>
+        <v>0</v>
       </c>
       <c r="E83" s="6">
         <v>142324.9</v>
@@ -4397,7 +4415,7 @@
         <v>25</v>
       </c>
       <c r="D86" s="5">
-        <v>310.25</v>
+        <v>0</v>
       </c>
       <c r="E86" s="6">
         <v>47466.76</v>
@@ -4443,7 +4461,7 @@
         <v>21</v>
       </c>
       <c r="D88" s="5">
-        <v>21.5</v>
+        <v>0</v>
       </c>
       <c r="E88" s="6">
         <v>7153.5</v>
@@ -4466,7 +4484,7 @@
         <v>23</v>
       </c>
       <c r="D89" s="5">
-        <v>161.25</v>
+        <v>0</v>
       </c>
       <c r="E89" s="6">
         <v>25805.64</v>
@@ -4512,7 +4530,7 @@
         <v>25</v>
       </c>
       <c r="D91" s="5">
-        <v>103.5</v>
+        <v>0</v>
       </c>
       <c r="E91" s="6">
         <v>15735.26</v>
@@ -4590,7 +4608,7 @@
         <v>1471.5</v>
       </c>
       <c r="F2" s="5">
-        <v>1443</v>
+        <v>0</v>
       </c>
       <c r="G2" s="6">
         <v>236151.87</v>
@@ -4616,7 +4634,7 @@
         <v>2969.75</v>
       </c>
       <c r="F3" s="5">
-        <v>2831.75</v>
+        <v>0</v>
       </c>
       <c r="G3" s="6">
         <v>427553.81</v>
@@ -4642,7 +4660,7 @@
         <v>7108.75</v>
       </c>
       <c r="F4" s="5">
-        <v>7076.75</v>
+        <v>0</v>
       </c>
       <c r="G4" s="6">
         <v>1074404.2</v>
@@ -4772,7 +4790,7 @@
         <v>4259</v>
       </c>
       <c r="F9" s="5">
-        <v>4165.5</v>
+        <v>0</v>
       </c>
       <c r="G9" s="6">
         <v>643351.32</v>
@@ -4788,7 +4806,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D719"/>
+  <dimension ref="A1:D725"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -13611,13 +13629,13 @@
         <v>668</v>
       </c>
       <c r="B630" s="6">
-        <v>2970</v>
+        <v>3858.75</v>
       </c>
       <c r="C630" s="6">
         <v>4169.93</v>
       </c>
       <c r="D630" s="6">
-        <v>-1199.93</v>
+        <v>-311.18</v>
       </c>
     </row>
     <row r="631">
@@ -14864,6 +14882,90 @@
       </c>
       <c r="D719" s="6">
         <v>0</v>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" s="0" t="s">
+        <v>758</v>
+      </c>
+      <c r="B720" s="6">
+        <v>2970</v>
+      </c>
+      <c r="C720" s="6">
+        <v>0</v>
+      </c>
+      <c r="D720" s="6">
+        <v>2970</v>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" s="0" t="s">
+        <v>759</v>
+      </c>
+      <c r="B721" s="6">
+        <v>-3858.75</v>
+      </c>
+      <c r="C721" s="6">
+        <v>0</v>
+      </c>
+      <c r="D721" s="6">
+        <v>-3858.75</v>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" s="0" t="s">
+        <v>760</v>
+      </c>
+      <c r="B722" s="6">
+        <v>535.5</v>
+      </c>
+      <c r="C722" s="6">
+        <v>0</v>
+      </c>
+      <c r="D722" s="6">
+        <v>535.5</v>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" s="0" t="s">
+        <v>761</v>
+      </c>
+      <c r="B723" s="6">
+        <v>-535.5</v>
+      </c>
+      <c r="C723" s="6">
+        <v>0</v>
+      </c>
+      <c r="D723" s="6">
+        <v>-535.5</v>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" s="0" t="s">
+        <v>762</v>
+      </c>
+      <c r="B724" s="6">
+        <v>1695.75</v>
+      </c>
+      <c r="C724" s="6">
+        <v>0</v>
+      </c>
+      <c r="D724" s="6">
+        <v>1695.75</v>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" s="0" t="s">
+        <v>763</v>
+      </c>
+      <c r="B725" s="6">
+        <v>-1695.75</v>
+      </c>
+      <c r="C725" s="6">
+        <v>0</v>
+      </c>
+      <c r="D725" s="6">
+        <v>-1695.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>